<commit_message>
Update the new n channel mosfet
</commit_message>
<xml_diff>
--- a/PCB_Rocket32_TRASIO/Rocket32_TRASIO_bom.xlsx
+++ b/PCB_Rocket32_TRASIO/Rocket32_TRASIO_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_Rocket32_TRASIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A1DC8-D260-48D2-8F19-94E2C5D8C614}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C88CA7-68AA-43D3-9340-0A736AE23DC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>C88711</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -53,7 +50,6 @@
         <sz val="11"/>
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>（</t>
     </r>
@@ -71,7 +67,6 @@
         <sz val="11"/>
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>）</t>
     </r>
@@ -133,10 +128,6 @@
     <t>IC3, IC5</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3, Q4</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>IC1, IC2</t>
   </si>
   <si>
@@ -161,10 +152,6 @@
     <t>C6185</t>
   </si>
   <si>
-    <t>BSH103,235</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>C53406</t>
   </si>
   <si>
@@ -172,6 +159,15 @@
   </si>
   <si>
     <t>SOT-223</t>
+  </si>
+  <si>
+    <t>Q5, Q6, Q7, Q8</t>
+  </si>
+  <si>
+    <t>2N7002K-7</t>
+  </si>
+  <si>
+    <t>C705095</t>
   </si>
 </sst>
 </file>
@@ -189,7 +185,6 @@
       <sz val="11"/>
       <color rgb="FFAFABAB"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -338,9 +333,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -351,6 +343,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +733,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -762,64 +757,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="16.5">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5">
         <v>1206</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>10</v>
+      <c r="D2" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
         <v>1206</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>25</v>
+      <c r="D3" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5">
         <v>1206</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>26</v>
+      <c r="D4" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5">
       <c r="A5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5">
         <v>1206</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>30</v>
+      <c r="D5" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5">
@@ -827,27 +822,27 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5">
         <v>1206</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>27</v>
+      <c r="D6" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5">
         <v>1206</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>28</v>
+      <c r="D7" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5">
@@ -855,122 +850,122 @@
         <v>330</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>1206</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>29</v>
+      <c r="D8" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:5" ht="15.75">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:5" ht="15.75">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:5" ht="15.75">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="15.75">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" ht="15.75">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="14"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" ht="15.75">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" ht="15.75">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" ht="15.75">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="15.75">
-      <c r="A22" s="14"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9"/>

</xml_diff>